<commit_message>
Update file read and rocksdb xlsx sheets.
Signed-off-by: Keshava Munegowda <keshava.gowda@gmail.com>
</commit_message>
<xml_diff>
--- a/samples/charts/sbk-file-read.xlsx
+++ b/samples/charts/sbk-file-read.xlsx
@@ -43,6 +43,13 @@
     <sheet name="Percentile_99.9" sheetId="35" state="visible" r:id="rId35"/>
     <sheet name="Percentile_99.95" sheetId="36" state="visible" r:id="rId36"/>
     <sheet name="Percentile_99.99" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="Total_Percentiles_1" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="Total_Percentiles_2" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="Total_MB" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="Total_Throughput_MB" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="Total_Throughput_Records" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="Total_Avg_Latency" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="Total_Max_Latency" sheetId="44" state="visible" r:id="rId44"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3548,6 +3555,658 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Percentiles</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1_FILE_2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'T1'!$Y$1:$AD$1</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'T1'!$Y$2:$AD$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Percentiles</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Latency time in NANOSECONDS</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Percentiles</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1_FILE_2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'T1'!$AD$1:$AS$1</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'T1'!$AD$2:$AS$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Percentiles</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Latency time in NANOSECONDS</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Mega Bytes Reading</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-MB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$N$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Throughput Variations in Mega Bytes / Seconds</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-MB/Sec</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$Q$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Throughput in MB/Sec</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Throughput Variations in Records / Seconds</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-Records/Sec</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$P$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Throughput in Records/Sec</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Average Latency Comparison</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-AvgLatency</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$R$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Average Latency</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
@@ -3665,6 +4324,111 @@
                 </a:pPr>
                 <a:r>
                   <a:t>Latency time in NANOSECONDS</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Max Latency Comparison</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-MaxLatency</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$S$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Max Latency</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -5639,6 +6403,141 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing35.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing36.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing37.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing38.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing39.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -5649,6 +6548,60 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="25200000" cy="25200000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing40.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing41.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -10896,6 +11849,44 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -10924,7 +11915,7 @@
     <row r="8">
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>SBK Version : 0.96</t>
+          <t>SBK Version : 0.991</t>
         </is>
       </c>
     </row>
@@ -10961,6 +11952,101 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add the graphs for write and read pending records and MBs
Signed-off-by: Keshava Munegowda <keshava.gowda@gmail.com>
</commit_message>
<xml_diff>
--- a/samples/charts/sbk-file-read.xlsx
+++ b/samples/charts/sbk-file-read.xlsx
@@ -47,14 +47,16 @@
     <sheet name="Percentile_99.9" sheetId="39" state="visible" r:id="rId39"/>
     <sheet name="Percentile_99.95" sheetId="40" state="visible" r:id="rId40"/>
     <sheet name="Percentile_99.99" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="Total_Percentiles_1" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="Total_Percentiles_2" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="Total_MB" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="Total_Throughput_MB" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="Total_Throughput_Records" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="Total_Min_Latency" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet name="Total_Avg_Latency" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet name="Total_Max_Latency" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="Write_Read_Records" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="Write_Read_MB" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="Total_Percentiles_1" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="Total_Percentiles_2" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="Total_MB" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="Total_Throughput_MB" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="Total_Throughput_Records" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="Total_Min_Latency" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="Total_Avg_Latency" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="Total_Max_Latency" sheetId="51" state="visible" r:id="rId51"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4166,6 +4168,739 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:t>Write and Read Records Variations</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>R1-FILE-WriteRequestRecords</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$N$2:$N$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>R1-FILE-ReadRequestRecords</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$R$2:$R$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>R1-FILE-WriteResponsePendingRecords</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$V$2:$V$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>R1-FILE-ReadResponsePendingRecords</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$X$2:$X$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>R1-FILE-WriteReadRequestPendingRecords</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$Z$2:$Z$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>R1-FILE-Records</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AC$2:$AC$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Intervals</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Write and Read Records</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Write and Read MBs Variations</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>R1-FILE-WriteRequestMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$M$2:$M$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>R1-FILE-ReadRequestMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$Q$2:$Q$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>R1-FILE-WriteResponsePendingMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$U$2:$U$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>R1-FILE-ReadResponsePendingMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$W$2:$W$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>R1-FILE-WriteReadRequestPendingMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$Y$2:$Y$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>R1-FILE-Records</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AC$2:$AC$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Intervals</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Write and Read MBs</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Latency Variations</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>R1-FILE-Percentile_5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AN$2:$AN$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>R1-FILE-Percentile_10</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AO$2:$AO$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>R1-FILE-Percentile_20</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AP$2:$AP$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>R1-FILE-Percentile_25</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AQ$2:$AQ$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>R1-FILE-Percentile_30</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AR$2:$AR$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>R1-FILE-Percentile_40</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AS$2:$AS$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>R1-FILE-Percentile_50</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AT$2:$AT$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Intervals</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Latency time in NANOSECONDS</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
               <a:t>Total Percentiles</a:t>
             </a:r>
           </a:p>
@@ -4270,7 +5005,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -4386,7 +5121,790 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Mega Bytes Reading</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-WriteRequestMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$M$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>T1-FILE-ReadRequestMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$Q$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>T1-FILE-WriteResponsePendingMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$U$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>T1-FILE-ReadResponsePendingMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$W$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>T1-FILE-WriteReadRequestPendingMB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$Y$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>T1-FILE-MB</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$AB$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Throughput Variations in Mega Bytes / Seconds</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-WriteRequestMB/Sec</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$P$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>T1-FILE-ReadRequestMB/Sec</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$T$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>T1-FILE-MB/Sec</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$AE$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Throughput in MB/Sec</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Throughput Variations in Records / Seconds</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-WriteRequestRecords/Sec</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$O$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>T1-FILE-ReadRequestRecords/Sec</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$S$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>T1-FILE-Records/Sec</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$AD$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Throughput in Records/Sec</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Min Latency Comparison</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-MinLatency</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$AG$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Min Latency</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Average Latency Comparison</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-AvgLatency</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$AF$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Average Latency</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Total Max Latency Comparison</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>T1-FILE-MaxLatency</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'T1'!$AH$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Reading</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total Max Latency</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -4411,7 +5929,7 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <v>R1-FILE-Percentile_5</v>
+            <v>R1-FILE-AvgLatency</v>
           </tx>
           <spPr>
             <a:ln>
@@ -4428,138 +5946,13 @@
           </marker>
           <val>
             <numRef>
-              <f>'R1'!$AN$2:$AN$13</f>
+              <f>'R1'!$AF$2:$AF$13</f>
             </numRef>
           </val>
         </ser>
         <ser>
           <idx val="1"/>
           <order val="1"/>
-          <tx>
-            <v>R1-FILE-Percentile_10</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AO$2:$AO$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>R1-FILE-Percentile_20</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AP$2:$AP$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <v>R1-FILE-Percentile_25</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AQ$2:$AQ$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <v>R1-FILE-Percentile_30</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AR$2:$AR$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <v>R1-FILE-Percentile_40</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AS$2:$AS$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
           <tx>
             <v>R1-FILE-Percentile_50</v>
           </tx>
@@ -4647,739 +6040,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Total Mega Bytes Reading</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>T1-FILE-WriteRequestMB</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$M$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>T1-FILE-ReadRequestMB</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$Q$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>T1-FILE-MB</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$AB$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Reading</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>MB</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Total Throughput Variations in Mega Bytes / Seconds</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>T1-FILE-WriteRequestMB/Sec</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$P$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>T1-FILE-ReadRequestMB/Sec</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$T$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>T1-FILE-MB/Sec</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$AE$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Reading</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Total Throughput in MB/Sec</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Total Throughput Variations in Records / Seconds</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>T1-FILE-WriteRequestRecords/Sec</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$O$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>T1-FILE-ReadRequestRecords/Sec</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$S$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>T1-FILE-Records/Sec</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$AD$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Reading</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Total Throughput in Records/Sec</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Total Min Latency Comparison</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>T1-FILE-MinLatency</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$AG$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Reading</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Total Min Latency</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Total Average Latency Comparison</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>T1-FILE-AvgLatency</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$AF$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Reading</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Total Average Latency</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Total Max Latency Comparison</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>T1-FILE-MaxLatency</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'T1'!$AH$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Reading</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Total Max Latency</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -5404,7 +6065,7 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <v>R1-FILE-AvgLatency</v>
+            <v>R1-FILE-Percentile_50</v>
           </tx>
           <spPr>
             <a:ln>
@@ -5421,13 +6082,846 @@
           </marker>
           <val>
             <numRef>
-              <f>'R1'!$AF$2:$AF$13</f>
+              <f>'R1'!$AT$2:$AT$13</f>
             </numRef>
           </val>
         </ser>
         <ser>
           <idx val="1"/>
           <order val="1"/>
+          <tx>
+            <v>R1-FILE-Percentile_60</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AU$2:$AU$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>R1-FILE-Percentile_70</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AV$2:$AV$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>R1-FILE-Percentile_75</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AW$2:$AW$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>R1-FILE-Percentile_80</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AX$2:$AX$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>R1-FILE-Percentile_90</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AY$2:$AY$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Intervals</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Latency time in NANOSECONDS</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Latency Variations</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>R1-FILE-Percentile_92.5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AZ$2:$AZ$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>R1-FILE-Percentile_95</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BA$2:$BA$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>R1-FILE-Percentile_97.5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BB$2:$BB$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>R1-FILE-Percentile_99</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BC$2:$BC$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>R1-FILE-Percentile_99.25</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BD$2:$BD$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>R1-FILE-Percentile_99.5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BE$2:$BE$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>R1-FILE-Percentile_99.75</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BF$2:$BF$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>R1-FILE-Percentile_99.9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BG$2:$BG$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>R1-FILE-Percentile_99.95</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BH$2:$BH$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="9"/>
+          <order val="9"/>
+          <tx>
+            <v>R1-FILE-Percentile_99.99</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$BI$2:$BI$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Intervals</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Latency time in NANOSECONDS</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Latency Variations</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>R1-FILE-MinLatency</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AG$2:$AG$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>R1-FILE-Percentile_5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AN$2:$AN$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Intervals</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Latency time in NANOSECONDS</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Latency Variations</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>R1-FILE-Percentile_5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AN$2:$AN$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>R1-FILE-Percentile_10</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AO$2:$AO$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>R1-FILE-Percentile_20</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AP$2:$AP$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>R1-FILE-Percentile_25</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AQ$2:$AQ$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>R1-FILE-Percentile_30</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AR$2:$AR$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>R1-FILE-Percentile_40</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'R1'!$AS$2:$AS$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
           <tx>
             <v>R1-FILE-Percentile_50</v>
           </tx>
@@ -5515,975 +7009,6 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Latency Variations</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>R1-FILE-Percentile_50</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AT$2:$AT$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>R1-FILE-Percentile_60</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AU$2:$AU$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>R1-FILE-Percentile_70</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AV$2:$AV$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <v>R1-FILE-Percentile_75</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AW$2:$AW$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <v>R1-FILE-Percentile_80</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AX$2:$AX$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <v>R1-FILE-Percentile_90</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AY$2:$AY$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Intervals</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Latency time in NANOSECONDS</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Latency Variations</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>R1-FILE-Percentile_92.5</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AZ$2:$AZ$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>R1-FILE-Percentile_95</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BA$2:$BA$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>R1-FILE-Percentile_97.5</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BB$2:$BB$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <v>R1-FILE-Percentile_99</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BC$2:$BC$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <v>R1-FILE-Percentile_99.25</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BD$2:$BD$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <v>R1-FILE-Percentile_99.5</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BE$2:$BE$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
-          <tx>
-            <v>R1-FILE-Percentile_99.75</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BF$2:$BF$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="7"/>
-          <order val="7"/>
-          <tx>
-            <v>R1-FILE-Percentile_99.9</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BG$2:$BG$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="8"/>
-          <order val="8"/>
-          <tx>
-            <v>R1-FILE-Percentile_99.95</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BH$2:$BH$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="9"/>
-          <order val="9"/>
-          <tx>
-            <v>R1-FILE-Percentile_99.99</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$BI$2:$BI$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Intervals</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Latency time in NANOSECONDS</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Latency Variations</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>R1-FILE-MinLatency</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AG$2:$AG$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>R1-FILE-Percentile_5</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AN$2:$AN$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Intervals</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Latency time in NANOSECONDS</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Latency Variations</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>R1-FILE-Percentile_5</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AN$2:$AN$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>R1-FILE-Percentile_10</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AO$2:$AO$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>R1-FILE-Percentile_20</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AP$2:$AP$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <v>R1-FILE-Percentile_25</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AQ$2:$AQ$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <v>R1-FILE-Percentile_30</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AR$2:$AR$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <v>R1-FILE-Percentile_40</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AS$2:$AS$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
-          <tx>
-            <v>R1-FILE-Percentile_50</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'R1'!$AT$2:$AT$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Intervals</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Latency time in NANOSECONDS</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -7538,6 +8063,60 @@
 </file>
 
 <file path=xl/drawings/drawing45.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing46.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing47.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -12160,6 +12739,44 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update sample xlsx sheets
Signed-off-by: Keshava Munegowda <keshava.gowda@gmail.com>
</commit_message>
<xml_diff>
--- a/samples/charts/sbk-file-read.xlsx
+++ b/samples/charts/sbk-file-read.xlsx
@@ -7010,29 +7010,48 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
     <from>
-      <col>4</col>
+      <col>10</col>
       <colOff>0</colOff>
-      <row>14</row>
+      <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="18000000" cy="9000000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
+    <to>
+      <col>19</col>
+      <colOff>285750</colOff>
+      <row>36</row>
+      <rowOff>71438</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Picture 1" descr="sbk-logo.png"/>
+        <cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="1143000"/>
+          <a:ext cx="5772150" cy="5786438"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
     <clientData/>
-  </oneCellAnchor>
+  </twoCellAnchor>
 </wsDr>
 </file>
 
@@ -7612,7 +7631,7 @@
       <row>14</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="25200000" cy="25200000"/>
+    <ext cx="18000000" cy="9000000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -8143,6 +8162,33 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing48.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="18000000" cy="9000000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -8233,7 +8279,7 @@
       <row>14</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="18000000" cy="9000000"/>
+    <ext cx="25200000" cy="25200000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -8562,7 +8608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -8576,6 +8622,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>